<commit_message>
ultima actualizacion (sin funcionar)
</commit_message>
<xml_diff>
--- a/salidas/latest-insiders-trading-Buy.xlsx
+++ b/salidas/latest-insiders-trading-Buy.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J35"/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,22 +476,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>SNDA</t>
+          <t>RHP</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Ribar Brandon</t>
+          <t>HASLAM WILLIAM E</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>President &amp; CEO</t>
+          <t>Director</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Jun 12</t>
+          <t>Jun 13</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -500,42 +500,42 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>23.85</v>
+        <v>100.28</v>
       </c>
       <c r="G2" t="n">
-        <v>4200</v>
+        <v>9972</v>
       </c>
       <c r="H2" t="n">
-        <v>100170</v>
+        <v>999989</v>
       </c>
       <c r="I2" t="n">
-        <v>312255</v>
+        <v>22790</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Jun 14 01:07 PM</t>
+          <t>Jun 14 02:40 PM</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>RZLT</t>
+          <t>NFBK</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ROBERTS BRIAN KENNETH</t>
+          <t>Fasanella David</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Chief Medical Officer</t>
+          <t>EVP</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Jun 14</t>
+          <t>Jun 13</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -544,42 +544,42 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>3.91</v>
+        <v>7.79</v>
       </c>
       <c r="G3" t="n">
-        <v>4300</v>
+        <v>1000</v>
       </c>
       <c r="H3" t="n">
-        <v>16828</v>
+        <v>7790</v>
       </c>
       <c r="I3" t="n">
-        <v>54352</v>
+        <v>4000</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Jun 14 12:51 PM</t>
+          <t>Jun 14 02:33 PM</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>RZLT</t>
+          <t>SR</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>ROBERTS BRIAN KENNETH</t>
+          <t>Rasche Steven P</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Chief Medical Officer</t>
+          <t>Executive Vice President</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Jun 14</t>
+          <t>Jun 13</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -588,42 +588,42 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>3.91</v>
+        <v>23.83</v>
       </c>
       <c r="G4" t="n">
-        <v>3300</v>
+        <v>4500</v>
       </c>
       <c r="H4" t="n">
-        <v>12916</v>
+        <v>107235</v>
       </c>
       <c r="I4" t="n">
-        <v>13000</v>
+        <v>16500</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Jun 14 12:51 PM</t>
+          <t>Jun 14 02:29 PM</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>GLBZ</t>
+          <t>NFBK</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Hanna Mark Christopher</t>
+          <t>Kulkarni Rachana A</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>President and CEO</t>
+          <t>Director</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Jun 12</t>
+          <t>Jun 13</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -632,37 +632,37 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>3.75</v>
+        <v>7.92</v>
       </c>
       <c r="G5" t="n">
-        <v>541</v>
+        <v>10000</v>
       </c>
       <c r="H5" t="n">
-        <v>2029</v>
+        <v>79221</v>
       </c>
       <c r="I5" t="n">
-        <v>4141</v>
+        <v>14057</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Jun 14 12:41 PM</t>
+          <t>Jun 14 02:26 PM</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>RRBI</t>
+          <t>HQL</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Crowell Michael D.</t>
+          <t>Saba Capital Management, L.P.</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Director</t>
+          <t>10% Owner</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -676,37 +676,37 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>46.15</v>
+        <v>13.88</v>
       </c>
       <c r="G6" t="n">
-        <v>1000</v>
+        <v>2400</v>
       </c>
       <c r="H6" t="n">
-        <v>46150</v>
+        <v>33312</v>
       </c>
       <c r="I6" t="n">
-        <v>14330</v>
+        <v>3407612</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Jun 14 12:39 PM</t>
+          <t>Jun 14 01:59 PM</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>RRBI</t>
+          <t>HQL</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Crowell Michael D.</t>
+          <t>Saba Capital Management, L.P.</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Director</t>
+          <t>10% Owner</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -720,42 +720,42 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>46.31</v>
+        <v>13.82</v>
       </c>
       <c r="G7" t="n">
-        <v>1000</v>
+        <v>8467</v>
       </c>
       <c r="H7" t="n">
-        <v>46310</v>
+        <v>117014</v>
       </c>
       <c r="I7" t="n">
-        <v>17350</v>
+        <v>3416079</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Jun 14 12:39 PM</t>
+          <t>Jun 14 01:59 PM</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>MSBI</t>
+          <t>SOFI</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>McDonnell Jeffrey M</t>
+          <t>Noto Anthony</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Director</t>
+          <t>Chief Executive Officer</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Jun 13</t>
+          <t>Jun 14</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -764,42 +764,42 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>21.8</v>
+        <v>6.48</v>
       </c>
       <c r="G8" t="n">
-        <v>2290</v>
+        <v>30715</v>
       </c>
       <c r="H8" t="n">
-        <v>49922</v>
+        <v>199110</v>
       </c>
       <c r="I8" t="n">
-        <v>24245</v>
+        <v>8121844</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Jun 14 12:35 PM</t>
+          <t>Jun 14 01:50 PM</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>RZLT</t>
+          <t>SNDA</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Evans Daron</t>
+          <t>Ribar Brandon</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>CFO</t>
+          <t>President &amp; CEO</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Jun 14</t>
+          <t>Jun 12</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -808,42 +808,42 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>4.04</v>
+        <v>23.85</v>
       </c>
       <c r="G9" t="n">
-        <v>40000</v>
+        <v>4200</v>
       </c>
       <c r="H9" t="n">
-        <v>161568</v>
+        <v>100170</v>
       </c>
       <c r="I9" t="n">
-        <v>40000</v>
+        <v>312255</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>Jun 14 12:06 PM</t>
+          <t>Jun 14 01:07 PM</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>RCG</t>
+          <t>RZLT</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>STAHL MURRAY</t>
+          <t>ROBERTS BRIAN KENNETH</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>President and CEO</t>
+          <t>Chief Medical Officer</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Jun 13</t>
+          <t>Jun 14</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -852,42 +852,42 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>1.65</v>
+        <v>3.91</v>
       </c>
       <c r="G10" t="n">
-        <v>14</v>
+        <v>4300</v>
       </c>
       <c r="H10" t="n">
-        <v>23</v>
+        <v>16828</v>
       </c>
       <c r="I10" t="n">
-        <v>5206</v>
+        <v>54352</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Jun 14 11:39 AM</t>
+          <t>Jun 14 12:51 PM</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>RCG</t>
+          <t>RZLT</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>STAHL MURRAY</t>
+          <t>ROBERTS BRIAN KENNETH</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>President and CEO</t>
+          <t>Chief Medical Officer</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Jun 13</t>
+          <t>Jun 14</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -896,37 +896,37 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>1.65</v>
+        <v>3.91</v>
       </c>
       <c r="G11" t="n">
-        <v>170</v>
+        <v>3300</v>
       </c>
       <c r="H11" t="n">
-        <v>280</v>
+        <v>12916</v>
       </c>
       <c r="I11" t="n">
-        <v>248532</v>
+        <v>13000</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Jun 14 11:39 AM</t>
+          <t>Jun 14 12:51 PM</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>NFBK</t>
+          <t>GLBZ</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Harrison Timothy C</t>
+          <t>Hanna Mark Christopher</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Director</t>
+          <t>President and CEO</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -940,32 +940,32 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>8.16</v>
+        <v>3.75</v>
       </c>
       <c r="G12" t="n">
-        <v>10000</v>
+        <v>541</v>
       </c>
       <c r="H12" t="n">
-        <v>81564</v>
+        <v>2029</v>
       </c>
       <c r="I12" t="n">
-        <v>77682</v>
+        <v>4141</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Jun 14 10:57 AM</t>
+          <t>Jun 14 12:41 PM</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>ANIX</t>
+          <t>RRBI</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Titterton Lewis H jr</t>
+          <t>Crowell Michael D.</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -975,7 +975,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Jun 13</t>
+          <t>Jun 12</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -984,37 +984,37 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>2.7</v>
+        <v>46.15</v>
       </c>
       <c r="G13" t="n">
-        <v>405</v>
+        <v>1000</v>
       </c>
       <c r="H13" t="n">
-        <v>1094</v>
+        <v>46150</v>
       </c>
       <c r="I13" t="n">
-        <v>856612</v>
+        <v>14330</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>Jun 14 09:56 AM</t>
+          <t>Jun 14 12:39 PM</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>TURN</t>
+          <t>RRBI</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Gift Alicia M</t>
+          <t>Crowell Michael D.</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Treasurer, Secretary</t>
+          <t>Director</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -1028,42 +1028,42 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>3.74</v>
+        <v>46.31</v>
       </c>
       <c r="G14" t="n">
         <v>1000</v>
       </c>
       <c r="H14" t="n">
-        <v>3740</v>
+        <v>46310</v>
       </c>
       <c r="I14" t="n">
-        <v>45465</v>
+        <v>17350</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>Jun 14 08:45 AM</t>
+          <t>Jun 14 12:39 PM</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>NRDY</t>
+          <t>MSBI</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Cohn Charles K.</t>
+          <t>McDonnell Jeffrey M</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Chief Executive Officer</t>
+          <t>Director</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Jun 12</t>
+          <t>Jun 13</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1072,42 +1072,42 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>1.8</v>
+        <v>21.8</v>
       </c>
       <c r="G15" t="n">
-        <v>500000</v>
+        <v>2290</v>
       </c>
       <c r="H15" t="n">
-        <v>900000</v>
+        <v>49922</v>
       </c>
       <c r="I15" t="n">
-        <v>1422976</v>
+        <v>24245</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>Jun 14 08:44 AM</t>
+          <t>Jun 14 12:35 PM</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>FTCI</t>
+          <t>RZLT</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Chatila Ahmad R</t>
+          <t>Evans Daron</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Director</t>
+          <t>CFO</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Jun 13</t>
+          <t>Jun 14</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1116,42 +1116,42 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>0.44</v>
+        <v>4.04</v>
       </c>
       <c r="G16" t="n">
-        <v>114726</v>
+        <v>40000</v>
       </c>
       <c r="H16" t="n">
-        <v>50479</v>
+        <v>161568</v>
       </c>
       <c r="I16" t="n">
-        <v>1082184</v>
+        <v>40000</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>Jun 14 08:44 AM</t>
+          <t>Jun 14 12:06 PM</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>CTCX</t>
+          <t>RCG</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Upton Richard A</t>
+          <t>STAHL MURRAY</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Director</t>
+          <t>President and CEO</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Jun 12</t>
+          <t>Jun 13</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1160,42 +1160,42 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>2.2</v>
+        <v>1.65</v>
       </c>
       <c r="G17" t="n">
-        <v>2000</v>
+        <v>14</v>
       </c>
       <c r="H17" t="n">
-        <v>4409</v>
+        <v>23</v>
       </c>
       <c r="I17" t="n">
-        <v>6400</v>
+        <v>5206</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>Jun 14 08:21 AM</t>
+          <t>Jun 14 11:39 AM</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>GENK</t>
+          <t>RCG</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Kim David Wook Jin</t>
+          <t>STAHL MURRAY</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Co-Chief Executive Officer</t>
+          <t>President and CEO</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Jun 12</t>
+          <t>Jun 13</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1204,42 +1204,42 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>10.69</v>
+        <v>1.65</v>
       </c>
       <c r="G18" t="n">
-        <v>2000</v>
+        <v>170</v>
       </c>
       <c r="H18" t="n">
-        <v>21380</v>
+        <v>280</v>
       </c>
       <c r="I18" t="n">
-        <v>166652</v>
+        <v>248532</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>Jun 13 09:31 PM</t>
+          <t>Jun 14 11:39 AM</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>NEXI</t>
+          <t>NFBK</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Jones Kristi</t>
+          <t>Harrison Timothy C</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>President and CEO</t>
+          <t>Director</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Jun 11</t>
+          <t>Jun 12</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1248,32 +1248,32 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>0.01</v>
+        <v>8.16</v>
       </c>
       <c r="G19" t="n">
-        <v>1</v>
+        <v>10000</v>
       </c>
       <c r="H19" t="n">
-        <v>0</v>
+        <v>81564</v>
       </c>
       <c r="I19" t="n">
-        <v>1</v>
+        <v>77682</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>Jun 13 07:58 PM</t>
+          <t>Jun 14 10:57 AM</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>FAT</t>
+          <t>ANIX</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>WIEDERHORN ANDREW</t>
+          <t>Titterton Lewis H jr</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1283,7 +1283,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Jun 11</t>
+          <t>Jun 13</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1292,37 +1292,37 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>14.21</v>
+        <v>2.7</v>
       </c>
       <c r="G20" t="n">
-        <v>646</v>
+        <v>405</v>
       </c>
       <c r="H20" t="n">
-        <v>9180</v>
+        <v>1094</v>
       </c>
       <c r="I20" t="n">
-        <v>1643</v>
+        <v>856612</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>Jun 13 07:57 PM</t>
+          <t>Jun 14 09:56 AM</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>VFC</t>
+          <t>TURN</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Carucci Richard</t>
+          <t>Gift Alicia M</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Director</t>
+          <t>Treasurer, Secretary</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1336,37 +1336,37 @@
         </is>
       </c>
       <c r="F21" t="n">
-        <v>13.78</v>
+        <v>3.74</v>
       </c>
       <c r="G21" t="n">
-        <v>25000</v>
+        <v>1000</v>
       </c>
       <c r="H21" t="n">
-        <v>344495</v>
+        <v>3740</v>
       </c>
       <c r="I21" t="n">
-        <v>215130</v>
+        <v>45465</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>Jun 13 07:30 PM</t>
+          <t>Jun 14 08:45 AM</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>SPWH</t>
+          <t>NRDY</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Sansom Steven W.</t>
+          <t>Cohn Charles K.</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Director</t>
+          <t>Chief Executive Officer</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1380,42 +1380,42 @@
         </is>
       </c>
       <c r="F22" t="n">
-        <v>2.91</v>
+        <v>1.8</v>
       </c>
       <c r="G22" t="n">
-        <v>10000</v>
+        <v>500000</v>
       </c>
       <c r="H22" t="n">
-        <v>29135</v>
+        <v>900000</v>
       </c>
       <c r="I22" t="n">
-        <v>90000</v>
+        <v>1422976</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>Jun 13 07:12 PM</t>
+          <t>Jun 14 08:44 AM</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>DTC</t>
+          <t>FTCI</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>METZ CHRISTOPHER T</t>
+          <t>Chatila Ahmad R</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>President &amp; CEO</t>
+          <t>Director</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Jun 11</t>
+          <t>Jun 13</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1424,37 +1424,37 @@
         </is>
       </c>
       <c r="F23" t="n">
-        <v>1.94</v>
+        <v>0.44</v>
       </c>
       <c r="G23" t="n">
-        <v>52366</v>
+        <v>114726</v>
       </c>
       <c r="H23" t="n">
-        <v>101721</v>
+        <v>50479</v>
       </c>
       <c r="I23" t="n">
-        <v>152366</v>
+        <v>1082184</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Jun 13 06:55 PM</t>
+          <t>Jun 14 08:44 AM</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>DTC</t>
+          <t>CTCX</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>METZ CHRISTOPHER T</t>
+          <t>Upton Richard A</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>President &amp; CEO</t>
+          <t>Director</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1468,42 +1468,42 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>1.98</v>
+        <v>2.2</v>
       </c>
       <c r="G24" t="n">
-        <v>48324</v>
+        <v>2000</v>
       </c>
       <c r="H24" t="n">
-        <v>95662</v>
+        <v>4409</v>
       </c>
       <c r="I24" t="n">
-        <v>200690</v>
+        <v>6400</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>Jun 13 06:55 PM</t>
+          <t>Jun 14 08:21 AM</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>DTC</t>
+          <t>GENK</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>METZ CHRISTOPHER T</t>
+          <t>Kim David Wook Jin</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>President &amp; CEO</t>
+          <t>Co-Chief Executive Officer</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Jun 13</t>
+          <t>Jun 12</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1512,42 +1512,42 @@
         </is>
       </c>
       <c r="F25" t="n">
-        <v>1.97</v>
+        <v>10.69</v>
       </c>
       <c r="G25" t="n">
-        <v>49310</v>
+        <v>2000</v>
       </c>
       <c r="H25" t="n">
-        <v>97234</v>
+        <v>21380</v>
       </c>
       <c r="I25" t="n">
-        <v>250000</v>
+        <v>166652</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>Jun 13 06:55 PM</t>
+          <t>Jun 13 09:31 PM</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>ZOM</t>
+          <t>NEXI</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Klass Russell Kevin</t>
+          <t>Jones Kristi</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Vice President of Sales</t>
+          <t>President and CEO</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Jun 12</t>
+          <t>Jun 11</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1556,32 +1556,32 @@
         </is>
       </c>
       <c r="F26" t="n">
-        <v>0.16</v>
+        <v>0.01</v>
       </c>
       <c r="G26" t="n">
-        <v>299993</v>
+        <v>1</v>
       </c>
       <c r="H26" t="n">
-        <v>46529</v>
+        <v>0</v>
       </c>
       <c r="I26" t="n">
-        <v>2000050</v>
+        <v>1</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Jun 13 06:32 PM</t>
+          <t>Jun 13 07:58 PM</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>FF</t>
+          <t>FAT</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>KRUSZEWSKI RONALD J</t>
+          <t>WIEDERHORN ANDREW</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1600,32 +1600,32 @@
         </is>
       </c>
       <c r="F27" t="n">
-        <v>4.5</v>
+        <v>14.21</v>
       </c>
       <c r="G27" t="n">
-        <v>8544</v>
+        <v>646</v>
       </c>
       <c r="H27" t="n">
-        <v>38448</v>
+        <v>9180</v>
       </c>
       <c r="I27" t="n">
-        <v>8544</v>
+        <v>1643</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>Jun 13 06:14 PM</t>
+          <t>Jun 13 07:57 PM</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>FF</t>
+          <t>VFC</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>KRUSZEWSKI RONALD J</t>
+          <t>Carucci Richard</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1635,7 +1635,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Jun 12</t>
+          <t>Jun 13</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -1644,32 +1644,32 @@
         </is>
       </c>
       <c r="F28" t="n">
-        <v>4.57</v>
+        <v>13.78</v>
       </c>
       <c r="G28" t="n">
-        <v>41098</v>
+        <v>25000</v>
       </c>
       <c r="H28" t="n">
-        <v>187818</v>
+        <v>344495</v>
       </c>
       <c r="I28" t="n">
-        <v>49642</v>
+        <v>215130</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>Jun 13 06:14 PM</t>
+          <t>Jun 13 07:30 PM</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>FF</t>
+          <t>SPWH</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>KRUSZEWSKI RONALD J</t>
+          <t>Sansom Steven W.</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1679,7 +1679,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Jun 13</t>
+          <t>Jun 12</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -1688,37 +1688,37 @@
         </is>
       </c>
       <c r="F29" t="n">
-        <v>4.6</v>
+        <v>2.91</v>
       </c>
       <c r="G29" t="n">
-        <v>50358</v>
+        <v>10000</v>
       </c>
       <c r="H29" t="n">
-        <v>231647</v>
+        <v>29135</v>
       </c>
       <c r="I29" t="n">
-        <v>100000</v>
+        <v>90000</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>Jun 13 06:14 PM</t>
+          <t>Jun 13 07:12 PM</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>ACRS</t>
+          <t>DTC</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Leonard Braden Michael</t>
+          <t>METZ CHRISTOPHER T</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>10% Owner</t>
+          <t>President &amp; CEO</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1732,37 +1732,37 @@
         </is>
       </c>
       <c r="F30" t="n">
-        <v>1.08</v>
+        <v>1.94</v>
       </c>
       <c r="G30" t="n">
-        <v>1000000</v>
+        <v>52366</v>
       </c>
       <c r="H30" t="n">
-        <v>1080000</v>
+        <v>101721</v>
       </c>
       <c r="I30" t="n">
-        <v>10395934</v>
+        <v>152366</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>Jun 13 06:04 PM</t>
+          <t>Jun 13 06:55 PM</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>ACRS</t>
+          <t>DTC</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Leonard Braden Michael</t>
+          <t>METZ CHRISTOPHER T</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>10% Owner</t>
+          <t>President &amp; CEO</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1776,37 +1776,37 @@
         </is>
       </c>
       <c r="F31" t="n">
-        <v>1.14</v>
+        <v>1.98</v>
       </c>
       <c r="G31" t="n">
-        <v>82579</v>
+        <v>48324</v>
       </c>
       <c r="H31" t="n">
-        <v>94140</v>
+        <v>95662</v>
       </c>
       <c r="I31" t="n">
-        <v>10478513</v>
+        <v>200690</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>Jun 13 06:04 PM</t>
+          <t>Jun 13 06:55 PM</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>ACRS</t>
+          <t>DTC</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Leonard Braden Michael</t>
+          <t>METZ CHRISTOPHER T</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>10% Owner</t>
+          <t>President &amp; CEO</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1820,42 +1820,42 @@
         </is>
       </c>
       <c r="F32" t="n">
-        <v>1.15</v>
+        <v>1.97</v>
       </c>
       <c r="G32" t="n">
-        <v>528621</v>
+        <v>49310</v>
       </c>
       <c r="H32" t="n">
-        <v>607757</v>
+        <v>97234</v>
       </c>
       <c r="I32" t="n">
-        <v>11007134</v>
+        <v>250000</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Jun 13 06:04 PM</t>
+          <t>Jun 13 06:55 PM</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>UBFO</t>
+          <t>ZOM</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>GILL JAGROOP</t>
+          <t>Klass Russell Kevin</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Director</t>
+          <t>Vice President of Sales</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Jun 11</t>
+          <t>Jun 12</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -1864,42 +1864,42 @@
         </is>
       </c>
       <c r="F33" t="n">
-        <v>7.2</v>
+        <v>0.16</v>
       </c>
       <c r="G33" t="n">
-        <v>8255</v>
+        <v>299993</v>
       </c>
       <c r="H33" t="n">
-        <v>59436</v>
+        <v>46529</v>
       </c>
       <c r="I33" t="n">
-        <v>1079667</v>
+        <v>2000050</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Jun 13 06:00 PM</t>
+          <t>Jun 13 06:32 PM</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>CBU</t>
+          <t>FF</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Karaivanov Dimitar</t>
+          <t>KRUSZEWSKI RONALD J</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>President &amp; CEO</t>
+          <t>Director</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Jun 13</t>
+          <t>Jun 11</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -1908,64 +1908,328 @@
         </is>
       </c>
       <c r="F34" t="n">
-        <v>43.52</v>
+        <v>4.5</v>
       </c>
       <c r="G34" t="n">
-        <v>1000</v>
+        <v>8544</v>
       </c>
       <c r="H34" t="n">
-        <v>43520</v>
+        <v>38448</v>
       </c>
       <c r="I34" t="n">
-        <v>19653</v>
+        <v>8544</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>Jun 13 05:37 PM</t>
+          <t>Jun 13 06:14 PM</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>GXO</t>
+          <t>FF</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Wilson Malcolm</t>
+          <t>KRUSZEWSKI RONALD J</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Chief Executive Officer</t>
+          <t>Director</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
+          <t>Jun 12</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="F35" t="n">
+        <v>4.57</v>
+      </c>
+      <c r="G35" t="n">
+        <v>41098</v>
+      </c>
+      <c r="H35" t="n">
+        <v>187818</v>
+      </c>
+      <c r="I35" t="n">
+        <v>49642</v>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>Jun 13 06:14 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>FF</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>KRUSZEWSKI RONALD J</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Director</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Jun 13</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="F36" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="G36" t="n">
+        <v>50358</v>
+      </c>
+      <c r="H36" t="n">
+        <v>231647</v>
+      </c>
+      <c r="I36" t="n">
+        <v>100000</v>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>Jun 13 06:14 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>ACRS</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Leonard Braden Michael</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>10% Owner</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
           <t>Jun 11</t>
         </is>
       </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>Buy</t>
-        </is>
-      </c>
-      <c r="F35" t="n">
-        <v>49.95</v>
-      </c>
-      <c r="G35" t="n">
-        <v>10000</v>
-      </c>
-      <c r="H35" t="n">
-        <v>499500</v>
-      </c>
-      <c r="I35" t="n">
-        <v>100814</v>
-      </c>
-      <c r="J35" t="inlineStr">
-        <is>
-          <t>Jun 13 05:27 PM</t>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="F37" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="G37" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="H37" t="n">
+        <v>1080000</v>
+      </c>
+      <c r="I37" t="n">
+        <v>10395934</v>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>Jun 13 06:04 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>ACRS</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Leonard Braden Michael</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>10% Owner</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Jun 12</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="F38" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="G38" t="n">
+        <v>82579</v>
+      </c>
+      <c r="H38" t="n">
+        <v>94140</v>
+      </c>
+      <c r="I38" t="n">
+        <v>10478513</v>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>Jun 13 06:04 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>ACRS</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Leonard Braden Michael</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>10% Owner</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Jun 13</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="F39" t="n">
+        <v>1.15</v>
+      </c>
+      <c r="G39" t="n">
+        <v>528621</v>
+      </c>
+      <c r="H39" t="n">
+        <v>607757</v>
+      </c>
+      <c r="I39" t="n">
+        <v>11007134</v>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>Jun 13 06:04 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>UBFO</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>GILL JAGROOP</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Director</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Jun 11</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="F40" t="n">
+        <v>7.2</v>
+      </c>
+      <c r="G40" t="n">
+        <v>8255</v>
+      </c>
+      <c r="H40" t="n">
+        <v>59436</v>
+      </c>
+      <c r="I40" t="n">
+        <v>1079667</v>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>Jun 13 06:00 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>CBU</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Karaivanov Dimitar</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>President &amp; CEO</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Jun 13</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="F41" t="n">
+        <v>43.52</v>
+      </c>
+      <c r="G41" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H41" t="n">
+        <v>43520</v>
+      </c>
+      <c r="I41" t="n">
+        <v>19653</v>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>Jun 13 05:37 PM</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
readme y creacion salidas si no existe
</commit_message>
<xml_diff>
--- a/salidas/latest-insiders-trading-Buy.xlsx
+++ b/salidas/latest-insiders-trading-Buy.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,22 +476,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>GLSI</t>
+          <t>REFR</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Patel Snehal</t>
+          <t>Kaganowicz Alexander</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>CEO and CFO</t>
+          <t>Director</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Jun 13</t>
+          <t>Jun 14</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -500,42 +500,42 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>14.3</v>
+        <v>1.94</v>
       </c>
       <c r="G2" t="n">
-        <v>174825</v>
+        <v>2000</v>
       </c>
       <c r="H2" t="n">
-        <v>2499998</v>
+        <v>3880</v>
       </c>
       <c r="I2" t="n">
-        <v>5525602</v>
+        <v>164923</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Jun 17 06:10 AM</t>
+          <t>Jun 17 06:30 AM</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>OPAD</t>
+          <t>GLSI</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Sella Roberto Marco</t>
+          <t>Patel Snehal</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Director</t>
+          <t>CEO and CFO</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Jun 12</t>
+          <t>Jun 13</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -544,20 +544,20 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>4.9</v>
+        <v>14.3</v>
       </c>
       <c r="G3" t="n">
-        <v>2735</v>
+        <v>174825</v>
       </c>
       <c r="H3" t="n">
-        <v>13402</v>
+        <v>2499998</v>
       </c>
       <c r="I3" t="n">
-        <v>3121185</v>
+        <v>5525602</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Jun 14 07:52 PM</t>
+          <t>Jun 17 06:10 AM</t>
         </is>
       </c>
     </row>
@@ -579,7 +579,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Jun 13</t>
+          <t>Jun 12</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -591,13 +591,13 @@
         <v>4.9</v>
       </c>
       <c r="G4" t="n">
-        <v>10000</v>
+        <v>2735</v>
       </c>
       <c r="H4" t="n">
-        <v>49000</v>
+        <v>13402</v>
       </c>
       <c r="I4" t="n">
-        <v>3131185</v>
+        <v>3121185</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -623,7 +623,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Jun 14</t>
+          <t>Jun 13</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -635,13 +635,13 @@
         <v>4.9</v>
       </c>
       <c r="G5" t="n">
-        <v>7698</v>
+        <v>10000</v>
       </c>
       <c r="H5" t="n">
-        <v>37720</v>
+        <v>49000</v>
       </c>
       <c r="I5" t="n">
-        <v>3138883</v>
+        <v>3131185</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -652,17 +652,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>SHEN</t>
+          <t>OPAD</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>FRENCH CHRISTOPHER E</t>
+          <t>Sella Roberto Marco</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>President &amp; CEO</t>
+          <t>Director</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -676,42 +676,42 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>15.79</v>
+        <v>4.9</v>
       </c>
       <c r="G6" t="n">
-        <v>5000</v>
+        <v>7698</v>
       </c>
       <c r="H6" t="n">
-        <v>78950</v>
+        <v>37720</v>
       </c>
       <c r="I6" t="n">
-        <v>84629</v>
+        <v>3138883</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Jun 14 07:41 PM</t>
+          <t>Jun 14 07:52 PM</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>DK</t>
+          <t>SHEN</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Marcogliese Richard J</t>
+          <t>FRENCH CHRISTOPHER E</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Director</t>
+          <t>President &amp; CEO</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Jun 12</t>
+          <t>Jun 14</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -720,37 +720,37 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>23.99</v>
+        <v>15.79</v>
       </c>
       <c r="G7" t="n">
-        <v>2750</v>
+        <v>5000</v>
       </c>
       <c r="H7" t="n">
-        <v>65972</v>
+        <v>78950</v>
       </c>
       <c r="I7" t="n">
-        <v>42863</v>
+        <v>84629</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Jun 14 07:19 PM</t>
+          <t>Jun 14 07:41 PM</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>LGF-A</t>
+          <t>DK</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Liberty 77 Capital L.P.</t>
+          <t>Marcogliese Richard J</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>10% Owner</t>
+          <t>Director</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -764,20 +764,20 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>8.01</v>
+        <v>23.99</v>
       </c>
       <c r="G8" t="n">
-        <v>275245</v>
+        <v>2750</v>
       </c>
       <c r="H8" t="n">
-        <v>2204988</v>
+        <v>65972</v>
       </c>
       <c r="I8" t="n">
-        <v>8631954</v>
+        <v>42863</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Jun 14 07:01 PM</t>
+          <t>Jun 14 07:19 PM</t>
         </is>
       </c>
     </row>
@@ -799,7 +799,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Jun 13</t>
+          <t>Jun 12</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -808,16 +808,16 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>8.140000000000001</v>
+        <v>8.01</v>
       </c>
       <c r="G9" t="n">
-        <v>324755</v>
+        <v>275245</v>
       </c>
       <c r="H9" t="n">
-        <v>2643408</v>
+        <v>2204988</v>
       </c>
       <c r="I9" t="n">
-        <v>8956709</v>
+        <v>8631954</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -843,7 +843,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Jun 14</t>
+          <t>Jun 13</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -852,16 +852,16 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>8.19</v>
+        <v>8.140000000000001</v>
       </c>
       <c r="G10" t="n">
-        <v>98858</v>
+        <v>324755</v>
       </c>
       <c r="H10" t="n">
-        <v>809350</v>
+        <v>2643408</v>
       </c>
       <c r="I10" t="n">
-        <v>9055567</v>
+        <v>8956709</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -872,7 +872,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>LGF-B</t>
+          <t>LGF-A</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -887,7 +887,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Jun 12</t>
+          <t>Jun 14</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -896,16 +896,16 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>8.01</v>
+        <v>8.19</v>
       </c>
       <c r="G11" t="n">
-        <v>275245</v>
+        <v>98858</v>
       </c>
       <c r="H11" t="n">
-        <v>2204988</v>
+        <v>809350</v>
       </c>
       <c r="I11" t="n">
-        <v>8631954</v>
+        <v>9055567</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -931,7 +931,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Jun 13</t>
+          <t>Jun 12</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -940,16 +940,16 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>8.140000000000001</v>
+        <v>8.01</v>
       </c>
       <c r="G12" t="n">
-        <v>324755</v>
+        <v>275245</v>
       </c>
       <c r="H12" t="n">
-        <v>2643408</v>
+        <v>2204988</v>
       </c>
       <c r="I12" t="n">
-        <v>8956709</v>
+        <v>8631954</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -975,7 +975,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Jun 14</t>
+          <t>Jun 13</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -984,16 +984,16 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>8.19</v>
+        <v>8.140000000000001</v>
       </c>
       <c r="G13" t="n">
-        <v>98858</v>
+        <v>324755</v>
       </c>
       <c r="H13" t="n">
-        <v>809350</v>
+        <v>2643408</v>
       </c>
       <c r="I13" t="n">
-        <v>9055567</v>
+        <v>8956709</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1004,22 +1004,22 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>PFX</t>
+          <t>LGF-B</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Lorber David A</t>
+          <t>Liberty 77 Capital L.P.</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>CHAIRMAN AND CEO</t>
+          <t>10% Owner</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Jun 12</t>
+          <t>Jun 14</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1028,20 +1028,20 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>44.98</v>
+        <v>8.19</v>
       </c>
       <c r="G14" t="n">
-        <v>628</v>
+        <v>98858</v>
       </c>
       <c r="H14" t="n">
-        <v>28245</v>
+        <v>809350</v>
       </c>
       <c r="I14" t="n">
-        <v>124961</v>
+        <v>9055567</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>Jun 14 06:56 PM</t>
+          <t>Jun 14 07:01 PM</t>
         </is>
       </c>
     </row>
@@ -1072,16 +1072,16 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>44.85</v>
+        <v>44.98</v>
       </c>
       <c r="G15" t="n">
-        <v>289</v>
+        <v>628</v>
       </c>
       <c r="H15" t="n">
-        <v>12961</v>
+        <v>28245</v>
       </c>
       <c r="I15" t="n">
-        <v>3289</v>
+        <v>124961</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1107,7 +1107,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Jun 14</t>
+          <t>Jun 12</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1116,16 +1116,16 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>45.08</v>
+        <v>44.85</v>
       </c>
       <c r="G16" t="n">
-        <v>64</v>
+        <v>289</v>
       </c>
       <c r="H16" t="n">
-        <v>2885</v>
+        <v>12961</v>
       </c>
       <c r="I16" t="n">
-        <v>125025</v>
+        <v>3289</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1136,22 +1136,22 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>TPB</t>
+          <t>PFX</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Frein Summer</t>
+          <t>Lorber David A</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Chief Revenue Officer</t>
+          <t>CHAIRMAN AND CEO</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Jun 13</t>
+          <t>Jun 14</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1160,42 +1160,42 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>30.96</v>
+        <v>45.08</v>
       </c>
       <c r="G17" t="n">
-        <v>2260</v>
+        <v>64</v>
       </c>
       <c r="H17" t="n">
-        <v>69970</v>
+        <v>2885</v>
       </c>
       <c r="I17" t="n">
-        <v>17203</v>
+        <v>125025</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>Jun 14 06:50 PM</t>
+          <t>Jun 14 06:56 PM</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>DALN</t>
+          <t>TPB</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>MURRAY MARY K</t>
+          <t>Frein Summer</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>President, Treasurer Secretary</t>
+          <t>Chief Revenue Officer</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Jun 12</t>
+          <t>Jun 13</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1204,20 +1204,20 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>3.76</v>
+        <v>30.96</v>
       </c>
       <c r="G18" t="n">
-        <v>1589</v>
+        <v>2260</v>
       </c>
       <c r="H18" t="n">
-        <v>5974</v>
+        <v>69970</v>
       </c>
       <c r="I18" t="n">
-        <v>7958</v>
+        <v>17203</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>Jun 14 06:40 PM</t>
+          <t>Jun 14 06:50 PM</t>
         </is>
       </c>
     </row>
@@ -1239,7 +1239,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Jun 13</t>
+          <t>Jun 12</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1248,16 +1248,16 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>3.83</v>
+        <v>3.76</v>
       </c>
       <c r="G19" t="n">
-        <v>5102</v>
+        <v>1589</v>
       </c>
       <c r="H19" t="n">
-        <v>19562</v>
+        <v>5974</v>
       </c>
       <c r="I19" t="n">
-        <v>13060</v>
+        <v>7958</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -1283,7 +1283,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Jun 14</t>
+          <t>Jun 13</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1292,16 +1292,16 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>3.77</v>
+        <v>3.83</v>
       </c>
       <c r="G20" t="n">
-        <v>309</v>
+        <v>5102</v>
       </c>
       <c r="H20" t="n">
-        <v>1165</v>
+        <v>19562</v>
       </c>
       <c r="I20" t="n">
-        <v>13369</v>
+        <v>13060</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -1312,17 +1312,17 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>RGEN</t>
+          <t>DALN</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Madaus Martin D</t>
+          <t>MURRAY MARY K</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Director</t>
+          <t>President, Treasurer Secretary</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1336,32 +1336,32 @@
         </is>
       </c>
       <c r="F21" t="n">
-        <v>124.94</v>
+        <v>3.77</v>
       </c>
       <c r="G21" t="n">
-        <v>1615</v>
+        <v>309</v>
       </c>
       <c r="H21" t="n">
-        <v>201776</v>
+        <v>1165</v>
       </c>
       <c r="I21" t="n">
-        <v>4613</v>
+        <v>13369</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>Jun 14 06:07 PM</t>
+          <t>Jun 14 06:40 PM</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>RKT</t>
+          <t>RGEN</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Rizik Matthew</t>
+          <t>Madaus Martin D</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1371,7 +1371,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Jun 13</t>
+          <t>Jun 14</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1380,20 +1380,20 @@
         </is>
       </c>
       <c r="F22" t="n">
-        <v>14.65</v>
+        <v>124.94</v>
       </c>
       <c r="G22" t="n">
-        <v>294</v>
+        <v>1615</v>
       </c>
       <c r="H22" t="n">
-        <v>4307</v>
+        <v>201776</v>
       </c>
       <c r="I22" t="n">
-        <v>704591</v>
+        <v>4613</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>Jun 14 06:02 PM</t>
+          <t>Jun 14 06:07 PM</t>
         </is>
       </c>
     </row>
@@ -1415,7 +1415,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Jun 14</t>
+          <t>Jun 13</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1424,16 +1424,16 @@
         </is>
       </c>
       <c r="F23" t="n">
-        <v>14.67</v>
+        <v>14.65</v>
       </c>
       <c r="G23" t="n">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="H23" t="n">
-        <v>4357</v>
+        <v>4307</v>
       </c>
       <c r="I23" t="n">
-        <v>704888</v>
+        <v>704591</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -1444,12 +1444,12 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>RGEN</t>
+          <t>RKT</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>BARTHELEMY NICOLAS</t>
+          <t>Rizik Matthew</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1468,20 +1468,20 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>125.45</v>
+        <v>14.67</v>
       </c>
       <c r="G24" t="n">
-        <v>1200</v>
+        <v>297</v>
       </c>
       <c r="H24" t="n">
-        <v>150540</v>
+        <v>4357</v>
       </c>
       <c r="I24" t="n">
-        <v>4668</v>
+        <v>704888</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>Jun 14 05:42 PM</t>
+          <t>Jun 14 06:02 PM</t>
         </is>
       </c>
     </row>
@@ -1493,12 +1493,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Hunt Anthony</t>
+          <t>BARTHELEMY NICOLAS</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Chief Executive Officer</t>
+          <t>Director</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1512,42 +1512,42 @@
         </is>
       </c>
       <c r="F25" t="n">
-        <v>124.08</v>
+        <v>125.45</v>
       </c>
       <c r="G25" t="n">
-        <v>2000</v>
+        <v>1200</v>
       </c>
       <c r="H25" t="n">
-        <v>248160</v>
+        <v>150540</v>
       </c>
       <c r="I25" t="n">
-        <v>165177</v>
+        <v>4668</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>Jun 14 05:41 PM</t>
+          <t>Jun 14 05:42 PM</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>SYPR</t>
+          <t>RGEN</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Convis Gary L</t>
+          <t>Hunt Anthony</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Director</t>
+          <t>Chief Executive Officer</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Jun 13</t>
+          <t>Jun 14</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1556,32 +1556,32 @@
         </is>
       </c>
       <c r="F26" t="n">
-        <v>1.92</v>
+        <v>124.08</v>
       </c>
       <c r="G26" t="n">
-        <v>20000</v>
+        <v>2000</v>
       </c>
       <c r="H26" t="n">
-        <v>38400</v>
+        <v>248160</v>
       </c>
       <c r="I26" t="n">
-        <v>449811</v>
+        <v>165177</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Jun 14 05:38 PM</t>
+          <t>Jun 14 05:41 PM</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>HTLD</t>
+          <t>SYPR</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>PRATT JAMES G</t>
+          <t>Convis Gary L</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1591,7 +1591,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Jun 12</t>
+          <t>Jun 13</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1600,37 +1600,37 @@
         </is>
       </c>
       <c r="F27" t="n">
-        <v>11.96</v>
+        <v>1.92</v>
       </c>
       <c r="G27" t="n">
-        <v>9000</v>
+        <v>20000</v>
       </c>
       <c r="H27" t="n">
-        <v>107619</v>
+        <v>38400</v>
       </c>
       <c r="I27" t="n">
-        <v>23429</v>
+        <v>449811</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>Jun 14 05:36 PM</t>
+          <t>Jun 14 05:38 PM</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>HLLY</t>
+          <t>HTLD</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Rubel Matthew E</t>
+          <t>PRATT JAMES G</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Exec. Chairman of the Board</t>
+          <t>Director</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1644,37 +1644,37 @@
         </is>
       </c>
       <c r="F28" t="n">
-        <v>3.39</v>
+        <v>11.96</v>
       </c>
       <c r="G28" t="n">
-        <v>14493</v>
+        <v>9000</v>
       </c>
       <c r="H28" t="n">
-        <v>49131</v>
+        <v>107619</v>
       </c>
       <c r="I28" t="n">
-        <v>169979</v>
+        <v>23429</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>Jun 14 05:24 PM</t>
+          <t>Jun 14 05:36 PM</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>TLPH</t>
+          <t>HLLY</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Angotti Vincent J.</t>
+          <t>Rubel Matthew E</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>CHIEF EXECUTIVE OFFICER</t>
+          <t>Exec. Chairman of the Board</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1688,20 +1688,20 @@
         </is>
       </c>
       <c r="F29" t="n">
-        <v>0.97</v>
+        <v>3.39</v>
       </c>
       <c r="G29" t="n">
-        <v>4126</v>
+        <v>14493</v>
       </c>
       <c r="H29" t="n">
-        <v>4013</v>
+        <v>49131</v>
       </c>
       <c r="I29" t="n">
-        <v>174932</v>
+        <v>169979</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>Jun 14 05:19 PM</t>
+          <t>Jun 14 05:24 PM</t>
         </is>
       </c>
     </row>
@@ -1723,7 +1723,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Jun 13</t>
+          <t>Jun 12</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -1735,13 +1735,13 @@
         <v>0.97</v>
       </c>
       <c r="G30" t="n">
-        <v>4570</v>
+        <v>4126</v>
       </c>
       <c r="H30" t="n">
-        <v>4438</v>
+        <v>4013</v>
       </c>
       <c r="I30" t="n">
-        <v>179502</v>
+        <v>174932</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -1767,27 +1767,71 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
+          <t>Jun 13</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="F31" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="G31" t="n">
+        <v>4570</v>
+      </c>
+      <c r="H31" t="n">
+        <v>4438</v>
+      </c>
+      <c r="I31" t="n">
+        <v>179502</v>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>Jun 14 05:19 PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>TLPH</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Angotti Vincent J.</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>CHIEF EXECUTIVE OFFICER</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
           <t>Jun 14</t>
         </is>
       </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>Buy</t>
-        </is>
-      </c>
-      <c r="F31" t="n">
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="F32" t="n">
         <v>1.08</v>
       </c>
-      <c r="G31" t="n">
+      <c r="G32" t="n">
         <v>1304</v>
       </c>
-      <c r="H31" t="n">
+      <c r="H32" t="n">
         <v>1404</v>
       </c>
-      <c r="I31" t="n">
+      <c r="I32" t="n">
         <v>180806</v>
       </c>
-      <c r="J31" t="inlineStr">
+      <c r="J32" t="inlineStr">
         <is>
           <t>Jun 14 05:19 PM</t>
         </is>

</xml_diff>